<commit_message>
reverting to original unbiased peak picks as much as possible since new method allowed for good fits on many more peaks
</commit_message>
<xml_diff>
--- a/paper_analysis/Results/Results (PW=False, rho=1.0, Flattop)/N_xi Fitted Parameters (rho=1.0, Flattop, PW=False, BW=50Hz).xlsx
+++ b/paper_analysis/Results/Results (PW=False, rho=1.0, Flattop)/N_xi Fitted Parameters (rho=1.0, Flattop, PW=False, BW=50Hz).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,34 +740,34 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2729.33349609375</v>
+        <v>3025.4150390625</v>
       </c>
       <c r="E7" t="n">
-        <v>14.25091630801473</v>
+        <v>20.89809237943588</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1062428160049067</v>
+        <v>0.6656618490556391</v>
       </c>
       <c r="G7" t="n">
-        <v>0.005221390617310338</v>
+        <v>0.006907512559305475</v>
       </c>
       <c r="H7" t="n">
-        <v>3.892628590715005e-05</v>
+        <v>0.0002200233159619352</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6276212533047167</v>
+        <v>0.5890790466590745</v>
       </c>
       <c r="J7" t="n">
-        <v>0.005702652896639536</v>
+        <v>0.04048123490850002</v>
       </c>
       <c r="K7" t="n">
-        <v>2.155687379634564e-06</v>
+        <v>5.858347886357718e-06</v>
       </c>
       <c r="L7" t="n">
-        <v>0.01496598639455782</v>
+        <v>0.02494331065759637</v>
       </c>
       <c r="M7" t="n">
-        <v>40.84716796875</v>
+        <v>75.4638671875</v>
       </c>
     </row>
     <row r="8">
@@ -875,34 +875,34 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2174.853515625</v>
+        <v>1814.17236328125</v>
       </c>
       <c r="E10" t="n">
-        <v>17.58882310624399</v>
+        <v>14.01485027664009</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4533511670646989</v>
+        <v>0.3706718128794821</v>
       </c>
       <c r="G10" t="n">
-        <v>0.008087359897978871</v>
+        <v>0.007725203271916109</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0002084513572098748</v>
+        <v>0.0002043200637281548</v>
       </c>
       <c r="I10" t="n">
-        <v>1.191966436023632</v>
+        <v>0.5000068988953382</v>
       </c>
       <c r="J10" t="n">
-        <v>0.03377602193061959</v>
+        <v>0.02966091844044146</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001839944359225175</v>
+        <v>2.933187586206043e-06</v>
       </c>
       <c r="L10" t="n">
-        <v>0.02095238095238095</v>
+        <v>0.02893424036281179</v>
       </c>
       <c r="M10" t="n">
-        <v>45.568359375</v>
+        <v>52.49169921875</v>
       </c>
     </row>
     <row r="11">
@@ -920,34 +920,34 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2497.8515625</v>
+        <v>2174.853515625</v>
       </c>
       <c r="E11" t="n">
-        <v>17.19645648666105</v>
+        <v>17.58882310624399</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2442314239366762</v>
+        <v>0.4533511670646989</v>
       </c>
       <c r="G11" t="n">
-        <v>0.006884498960958992</v>
+        <v>0.008087359897978871</v>
       </c>
       <c r="H11" t="n">
-        <v>9.777659633714771e-05</v>
+        <v>0.0002084513572098748</v>
       </c>
       <c r="I11" t="n">
-        <v>1.079681630028549</v>
+        <v>1.191966436023632</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01832986009724048</v>
+        <v>0.03377602193061959</v>
       </c>
       <c r="K11" t="n">
-        <v>3.225725581282323e-05</v>
+        <v>0.0001839944359225175</v>
       </c>
       <c r="L11" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.02095238095238095</v>
       </c>
       <c r="M11" t="n">
-        <v>47.3515625</v>
+        <v>45.568359375</v>
       </c>
     </row>
     <row r="12">
@@ -1133,91 +1133,91 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ALrearSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2804.69970703125</v>
+        <v>2417.10205078125</v>
       </c>
       <c r="E16" t="n">
-        <v>88.3585901946811</v>
+        <v>11.84479802408623</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5050242225391341</v>
+        <v>0.2696128683558961</v>
       </c>
       <c r="G16" t="n">
-        <v>0.03150376133786097</v>
+        <v>0.004900412880895028</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0001800635630520666</v>
+        <v>0.0001115438499043731</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2873848177380276</v>
+        <v>0.2874527503048795</v>
       </c>
       <c r="J16" t="n">
-        <v>0.001774536654292121</v>
+        <v>0.009480481296595997</v>
       </c>
       <c r="K16" t="n">
-        <v>2.626424328157188e-06</v>
+        <v>2.27906024824424e-06</v>
       </c>
       <c r="L16" t="n">
-        <v>0.08380952380952381</v>
+        <v>0.01496598639455782</v>
       </c>
       <c r="M16" t="n">
-        <v>235.060546875</v>
+        <v>36.17431640625</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ALrearSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2944.66552734375</v>
+        <v>2777.783203125</v>
       </c>
       <c r="E17" t="n">
-        <v>112.7838294385766</v>
+        <v>14.88026445029862</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5894286182731304</v>
+        <v>0.1524407274138239</v>
       </c>
       <c r="G17" t="n">
-        <v>0.03830106624717879</v>
+        <v>0.005356884739441996</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0002001682747326578</v>
+        <v>5.48785546842995e-05</v>
       </c>
       <c r="I17" t="n">
-        <v>0.5659013575728953</v>
+        <v>0.2084249425644493</v>
       </c>
       <c r="J17" t="n">
-        <v>0.003175768257435777</v>
+        <v>0.002588380669694693</v>
       </c>
       <c r="K17" t="n">
-        <v>1.114266955807588e-05</v>
+        <v>5.133608060689924e-07</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1047619047619048</v>
+        <v>0.01596371882086168</v>
       </c>
       <c r="M17" t="n">
-        <v>308.48876953125</v>
+        <v>44.34375</v>
       </c>
     </row>
     <row r="18">
@@ -1235,34 +1235,34 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3865.2099609375</v>
+        <v>2664.73388671875</v>
       </c>
       <c r="E18" t="n">
-        <v>187.1724350962789</v>
+        <v>25.6099289750788</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5929635328586602</v>
+        <v>0.8954081672797741</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04842490756980262</v>
+        <v>0.009610689120861474</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0001534104327711186</v>
+        <v>0.0003360216086651508</v>
       </c>
       <c r="I18" t="n">
-        <v>0.6122808224619363</v>
+        <v>0.1989686296376954</v>
       </c>
       <c r="J18" t="n">
-        <v>0.001957867042954829</v>
+        <v>0.009900790799493105</v>
       </c>
       <c r="K18" t="n">
-        <v>6.7356048573718e-06</v>
+        <v>6.646465132502183e-06</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1257142857142857</v>
+        <v>0.02993197278911565</v>
       </c>
       <c r="M18" t="n">
-        <v>485.9121093750001</v>
+        <v>79.7607421875</v>
       </c>
     </row>
     <row r="19">
@@ -1272,42 +1272,42 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2810.0830078125</v>
+        <v>2804.69970703125</v>
       </c>
       <c r="E19" t="n">
-        <v>159.0563848692604</v>
+        <v>88.3585901946811</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4094231827257127</v>
+        <v>0.5050242225391341</v>
       </c>
       <c r="G19" t="n">
-        <v>0.05660202365092314</v>
+        <v>0.03150376133786097</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0001456978963210154</v>
+        <v>0.0001800635630520666</v>
       </c>
       <c r="I19" t="n">
-        <v>0.6106819665582152</v>
+        <v>0.2873848177380276</v>
       </c>
       <c r="J19" t="n">
-        <v>0.001657271346758769</v>
+        <v>0.001774536654292121</v>
       </c>
       <c r="K19" t="n">
-        <v>4.958726786450073e-06</v>
+        <v>2.626424328157188e-06</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1546485260770975</v>
+        <v>0.08380952380952381</v>
       </c>
       <c r="M19" t="n">
-        <v>434.5751953125</v>
+        <v>235.060546875</v>
       </c>
     </row>
     <row r="20">
@@ -1317,42 +1317,42 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2341.73583984375</v>
+        <v>2944.66552734375</v>
       </c>
       <c r="E20" t="n">
-        <v>481.2123000325353</v>
+        <v>112.7838294385766</v>
       </c>
       <c r="F20" t="n">
-        <v>1.95413980325997</v>
+        <v>0.5894286182731304</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2054938442863153</v>
+        <v>0.03830106624717879</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0008344834502726654</v>
+        <v>0.0002001682747326578</v>
       </c>
       <c r="I20" t="n">
-        <v>1.12963301344575</v>
+        <v>0.5659013575728953</v>
       </c>
       <c r="J20" t="n">
-        <v>0.003839890097238593</v>
+        <v>0.003175768257435777</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0002223293862243911</v>
+        <v>1.114266955807588e-05</v>
       </c>
       <c r="L20" t="n">
-        <v>0.4709297052154195</v>
+        <v>0.1047619047619048</v>
       </c>
       <c r="M20" t="n">
-        <v>1102.79296875</v>
+        <v>308.48876953125</v>
       </c>
     </row>
     <row r="21">
@@ -1362,42 +1362,42 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4048.2421875</v>
+        <v>3865.2099609375</v>
       </c>
       <c r="E21" t="n">
-        <v>460.0213370230606</v>
+        <v>187.1724350962789</v>
       </c>
       <c r="F21" t="n">
-        <v>2.954926935351355</v>
+        <v>0.5929635328586602</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1136348359896787</v>
+        <v>0.04842490756980262</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0007299283981762406</v>
+        <v>0.0001534104327711186</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9376156448253929</v>
+        <v>0.6122808224619363</v>
       </c>
       <c r="J21" t="n">
-        <v>0.006094311819320653</v>
+        <v>0.001957867042954829</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0001466262973149197</v>
+        <v>6.7356048573718e-06</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2873469387755102</v>
+        <v>0.1257142857142857</v>
       </c>
       <c r="M21" t="n">
-        <v>1163.25</v>
+        <v>485.9121093750001</v>
       </c>
     </row>
     <row r="22">
@@ -1415,34 +1415,34 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5840.88134765625</v>
+        <v>2341.73583984375</v>
       </c>
       <c r="E22" t="n">
-        <v>294.9856749450948</v>
+        <v>481.2123000325353</v>
       </c>
       <c r="F22" t="n">
-        <v>1.37163524280064</v>
+        <v>1.95413980325997</v>
       </c>
       <c r="G22" t="n">
-        <v>0.05050362392029462</v>
+        <v>0.2054938442863153</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0002348336083476565</v>
+        <v>0.0008344834502726654</v>
       </c>
       <c r="I22" t="n">
-        <v>0.6821282846621883</v>
+        <v>1.12963301344575</v>
       </c>
       <c r="J22" t="n">
-        <v>0.003270002812562133</v>
+        <v>0.003839890097238593</v>
       </c>
       <c r="K22" t="n">
-        <v>1.82478511864518e-05</v>
+        <v>0.0002223293862243911</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1336961451247166</v>
+        <v>0.4709297052154195</v>
       </c>
       <c r="M22" t="n">
-        <v>780.9033203125</v>
+        <v>1102.79296875</v>
       </c>
     </row>
     <row r="23">
@@ -1452,42 +1452,42 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>732.12890625</v>
+        <v>5840.88134765625</v>
       </c>
       <c r="E23" t="n">
-        <v>219.4039453471672</v>
+        <v>294.9856749450948</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6358956789061395</v>
+        <v>1.37163524280064</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2996793918040538</v>
+        <v>0.05050362392029462</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0008685569897290741</v>
+        <v>0.0002348336083476565</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3256606079972586</v>
+        <v>0.6821282846621883</v>
       </c>
       <c r="J23" t="n">
-        <v>0.001243739004506885</v>
+        <v>0.003270002812562133</v>
       </c>
       <c r="K23" t="n">
-        <v>5.084957107542066e-06</v>
+        <v>1.82478511864518e-05</v>
       </c>
       <c r="L23" t="n">
-        <v>0.8680272108843538</v>
+        <v>0.1336961451247166</v>
       </c>
       <c r="M23" t="n">
-        <v>635.5078125</v>
+        <v>780.9033203125</v>
       </c>
     </row>
     <row r="24">
@@ -1497,42 +1497,42 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>985.14404296875</v>
+        <v>8311.81640625</v>
       </c>
       <c r="E24" t="n">
-        <v>411.5473593416629</v>
+        <v>840.0722721768307</v>
       </c>
       <c r="F24" t="n">
-        <v>2.511644915939776</v>
+        <v>5.778411880715729</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4177534871971181</v>
+        <v>0.101069637623991</v>
       </c>
       <c r="H24" t="n">
-        <v>0.002549520482680773</v>
+        <v>0.0006952044653405363</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2127470452341409</v>
+        <v>0.9146875902225527</v>
       </c>
       <c r="J24" t="n">
-        <v>0.001362827276667496</v>
+        <v>0.004870159551476776</v>
       </c>
       <c r="K24" t="n">
-        <v>1.895798727345385e-05</v>
+        <v>0.0002276337793343731</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9737868480725623</v>
+        <v>0.2195011337868481</v>
       </c>
       <c r="M24" t="n">
-        <v>959.3203125</v>
+        <v>1824.453125</v>
       </c>
     </row>
     <row r="25">
@@ -1542,42 +1542,42 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1636.5234375</v>
+        <v>8677.880859375</v>
       </c>
       <c r="E25" t="n">
-        <v>72.67268752654496</v>
+        <v>94.34958255388089</v>
       </c>
       <c r="F25" t="n">
-        <v>0.8219620585347209</v>
+        <v>2.538683061351535</v>
       </c>
       <c r="G25" t="n">
-        <v>0.04440675022507581</v>
+        <v>0.0108724219752282</v>
       </c>
       <c r="H25" t="n">
-        <v>0.000502261097946983</v>
+        <v>0.0002925464295362977</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1569031897804355</v>
+        <v>0.2817937922209833</v>
       </c>
       <c r="J25" t="n">
-        <v>0.001786450836843506</v>
+        <v>0.01030122978612125</v>
       </c>
       <c r="K25" t="n">
-        <v>4.488323932851304e-06</v>
+        <v>1.381919113908138e-05</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1067573696145125</v>
+        <v>0.04090702947845805</v>
       </c>
       <c r="M25" t="n">
-        <v>174.7109375</v>
+        <v>354.986328125</v>
       </c>
     </row>
     <row r="26">
@@ -1595,34 +1595,34 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2228.6865234375</v>
+        <v>732.12890625</v>
       </c>
       <c r="E26" t="n">
-        <v>336.6241596164451</v>
+        <v>219.4039453471672</v>
       </c>
       <c r="F26" t="n">
-        <v>1.835030340613512</v>
+        <v>0.6358956789061395</v>
       </c>
       <c r="G26" t="n">
-        <v>0.151041501833663</v>
+        <v>0.2996793918040538</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0008233685272988427</v>
+        <v>0.0008685569897290741</v>
       </c>
       <c r="I26" t="n">
-        <v>0.6695603821326709</v>
+        <v>0.3256606079972586</v>
       </c>
       <c r="J26" t="n">
-        <v>0.003494937339214901</v>
+        <v>0.001243739004506885</v>
       </c>
       <c r="K26" t="n">
-        <v>8.031796430238116e-05</v>
+        <v>5.084957107542066e-06</v>
       </c>
       <c r="L26" t="n">
-        <v>0.371156462585034</v>
+        <v>0.8680272108843538</v>
       </c>
       <c r="M26" t="n">
-        <v>827.1914062499999</v>
+        <v>635.5078125</v>
       </c>
     </row>
     <row r="27">
@@ -1632,42 +1632,42 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>LSrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>904.39453125</v>
+        <v>985.14404296875</v>
       </c>
       <c r="E27" t="n">
-        <v>181.6030294674161</v>
+        <v>411.5473593416629</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7443134424834201</v>
+        <v>2.511644915939776</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2008006718223022</v>
+        <v>0.4177534871971181</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0008229963989882542</v>
+        <v>0.002549520482680773</v>
       </c>
       <c r="I27" t="n">
-        <v>0.295894973176703</v>
+        <v>0.2127470452341409</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0009959021959020339</v>
+        <v>0.001362827276667496</v>
       </c>
       <c r="K27" t="n">
-        <v>1.681650732818304e-05</v>
+        <v>1.895798727345385e-05</v>
       </c>
       <c r="L27" t="n">
-        <v>0.4739229024943311</v>
+        <v>0.9737868480725623</v>
       </c>
       <c r="M27" t="n">
-        <v>428.61328125</v>
+        <v>959.3203125</v>
       </c>
     </row>
     <row r="28">
@@ -1677,42 +1677,42 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>LSrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1518.0908203125</v>
+        <v>1636.5234375</v>
       </c>
       <c r="E28" t="n">
-        <v>368.4028730034734</v>
+        <v>72.67268752654496</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5217499613791636</v>
+        <v>0.8219620585347209</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2426751206674429</v>
+        <v>0.04440675022507581</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0003436882394636713</v>
+        <v>0.000502261097946983</v>
       </c>
       <c r="I28" t="n">
-        <v>0.6181562129333856</v>
+        <v>0.1569031897804355</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0007284464263385937</v>
+        <v>0.001786450836843506</v>
       </c>
       <c r="K28" t="n">
-        <v>1.082495301871751e-05</v>
+        <v>4.488323932851304e-06</v>
       </c>
       <c r="L28" t="n">
-        <v>0.5926530612244898</v>
+        <v>0.1067573696145125</v>
       </c>
       <c r="M28" t="n">
-        <v>899.701171875</v>
+        <v>174.7109375</v>
       </c>
     </row>
     <row r="29">
@@ -1722,42 +1722,42 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>LSrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1674.20654296875</v>
+        <v>2228.6865234375</v>
       </c>
       <c r="E29" t="n">
-        <v>522.4434762486635</v>
+        <v>336.6241596164451</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7390236669104481</v>
+        <v>1.835030340613512</v>
       </c>
       <c r="G29" t="n">
-        <v>0.3120543749173576</v>
+        <v>0.151041501833663</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0004414172612179562</v>
+        <v>0.0008233685272988427</v>
       </c>
       <c r="I29" t="n">
-        <v>0.7513803364013724</v>
+        <v>0.6695603821326709</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0008459945309044197</v>
+        <v>0.003494937339214901</v>
       </c>
       <c r="K29" t="n">
-        <v>2.239812705725473e-05</v>
+        <v>8.031796430238116e-05</v>
       </c>
       <c r="L29" t="n">
-        <v>0.7492970521541951</v>
+        <v>0.371156462585034</v>
       </c>
       <c r="M29" t="n">
-        <v>1254.47802734375</v>
+        <v>827.1914062499999</v>
       </c>
     </row>
     <row r="30">
@@ -1775,169 +1775,169 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2040.27099609375</v>
+        <v>904.39453125</v>
       </c>
       <c r="E30" t="n">
-        <v>210.4506001278691</v>
+        <v>181.6030294674161</v>
       </c>
       <c r="F30" t="n">
-        <v>0.5763542799024319</v>
+        <v>0.7443134424834201</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1031483565324373</v>
+        <v>0.2008006718223022</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0002824890816003878</v>
+        <v>0.0008229963989882542</v>
       </c>
       <c r="I30" t="n">
-        <v>0.8358939323039025</v>
+        <v>0.295894973176703</v>
       </c>
       <c r="J30" t="n">
-        <v>0.002000888595176705</v>
+        <v>0.0009959021959020339</v>
       </c>
       <c r="K30" t="n">
-        <v>2.66339698612184e-05</v>
+        <v>1.681650732818304e-05</v>
       </c>
       <c r="L30" t="n">
-        <v>0.247437641723356</v>
+        <v>0.4739229024943311</v>
       </c>
       <c r="M30" t="n">
-        <v>504.83984375</v>
+        <v>428.61328125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>8009.765625</v>
+        <v>1518.0908203125</v>
       </c>
       <c r="E31" t="n">
-        <v>39.56021516831898</v>
+        <v>368.4028730034734</v>
       </c>
       <c r="F31" t="n">
-        <v>0.46711575285551</v>
+        <v>0.5217499613791636</v>
       </c>
       <c r="G31" t="n">
-        <v>0.004938997845934972</v>
+        <v>0.2426751206674429</v>
       </c>
       <c r="H31" t="n">
-        <v>5.831827980054161e-05</v>
+        <v>0.0003436882394636713</v>
       </c>
       <c r="I31" t="n">
-        <v>0.3298907438101564</v>
+        <v>0.6181562129333856</v>
       </c>
       <c r="J31" t="n">
-        <v>0.004930076339101207</v>
+        <v>0.0007284464263385937</v>
       </c>
       <c r="K31" t="n">
-        <v>1.368129640590637e-06</v>
+        <v>1.082495301871751e-05</v>
       </c>
       <c r="L31" t="n">
-        <v>0.015</v>
+        <v>0.5926530612244898</v>
       </c>
       <c r="M31" t="n">
-        <v>120.146484375</v>
+        <v>899.701171875</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8431.640625</v>
+        <v>2040.27099609375</v>
       </c>
       <c r="E32" t="n">
-        <v>33.95188442909585</v>
+        <v>210.4506001278691</v>
       </c>
       <c r="F32" t="n">
-        <v>0.6356775038384253</v>
+        <v>0.5763542799024319</v>
       </c>
       <c r="G32" t="n">
-        <v>0.004026723379128347</v>
+        <v>0.1031483565324373</v>
       </c>
       <c r="H32" t="n">
-        <v>7.539191150458043e-05</v>
+        <v>0.0002824890816003878</v>
       </c>
       <c r="I32" t="n">
-        <v>0.4084228789259367</v>
+        <v>0.8358939323039025</v>
       </c>
       <c r="J32" t="n">
-        <v>0.009073383355506844</v>
+        <v>0.002000888595176705</v>
       </c>
       <c r="K32" t="n">
-        <v>4.825068715576253e-06</v>
+        <v>2.66339698612184e-05</v>
       </c>
       <c r="L32" t="n">
-        <v>0.012</v>
+        <v>0.247437641723356</v>
       </c>
       <c r="M32" t="n">
-        <v>101.1796875</v>
+        <v>504.83984375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>7892.578125</v>
+        <v>2697.03369140625</v>
       </c>
       <c r="E33" t="n">
-        <v>43.9350953165799</v>
+        <v>31.42247898482017</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9972192019632076</v>
+        <v>0.6778334744375752</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00556663419997251</v>
+        <v>0.01165075508138584</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0001263489807981099</v>
+        <v>0.0002513255494721494</v>
       </c>
       <c r="I33" t="n">
-        <v>0.3713687639435128</v>
+        <v>0.3491989225251852</v>
       </c>
       <c r="J33" t="n">
-        <v>0.01129339804451088</v>
+        <v>0.01081760241943911</v>
       </c>
       <c r="K33" t="n">
-        <v>5.306494693467216e-06</v>
+        <v>9.159463069366274e-06</v>
       </c>
       <c r="L33" t="n">
-        <v>0.016</v>
+        <v>0.03591836734693878</v>
       </c>
       <c r="M33" t="n">
-        <v>126.28125</v>
+        <v>96.873046875</v>
       </c>
     </row>
     <row r="34">
@@ -1947,42 +1947,42 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>7500</v>
+        <v>4353.515625</v>
       </c>
       <c r="E34" t="n">
-        <v>37.42093375751286</v>
+        <v>26.71725345365265</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5786051692180033</v>
+        <v>1.62563614269226</v>
       </c>
       <c r="G34" t="n">
-        <v>0.004989457834335047</v>
+        <v>0.006136937536236052</v>
       </c>
       <c r="H34" t="n">
-        <v>7.714735589573378e-05</v>
+        <v>0.0003734076738709901</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2637212980789849</v>
+        <v>0.1393742050115217</v>
       </c>
       <c r="J34" t="n">
-        <v>0.005901294616173117</v>
+        <v>0.009294617188918301</v>
       </c>
       <c r="K34" t="n">
-        <v>1.020539795750622e-06</v>
+        <v>8.575156448300475e-06</v>
       </c>
       <c r="L34" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="M34" t="n">
-        <v>120</v>
+        <v>65.302734375</v>
       </c>
     </row>
     <row r="35">
@@ -1992,42 +1992,42 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>8835.9375</v>
+        <v>7453.125</v>
       </c>
       <c r="E35" t="n">
-        <v>43.38546643502074</v>
+        <v>39.74579289263069</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6609823171074566</v>
+        <v>0.9527090296496715</v>
       </c>
       <c r="G35" t="n">
-        <v>0.004910114680532851</v>
+        <v>0.005332768857711455</v>
       </c>
       <c r="H35" t="n">
-        <v>7.480613314743983e-05</v>
+        <v>0.0001278267880452389</v>
       </c>
       <c r="I35" t="n">
-        <v>0.4286776246064646</v>
+        <v>0.2627318458553665</v>
       </c>
       <c r="J35" t="n">
-        <v>0.008199907896277028</v>
+        <v>0.007581115877661915</v>
       </c>
       <c r="K35" t="n">
-        <v>3.410422038026642e-06</v>
+        <v>4.009940730980257e-06</v>
       </c>
       <c r="L35" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="M35" t="n">
-        <v>123.703125</v>
+        <v>111.796875</v>
       </c>
     </row>
     <row r="36">
@@ -2037,42 +2037,42 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>6034.68017578125</v>
+        <v>8431.640625</v>
       </c>
       <c r="E36" t="n">
-        <v>38.90591683588232</v>
+        <v>33.95188442909585</v>
       </c>
       <c r="F36" t="n">
-        <v>1.580104857260979</v>
+        <v>0.6356775038384253</v>
       </c>
       <c r="G36" t="n">
-        <v>0.006447055304110719</v>
+        <v>0.004026723379128347</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0002618373818056429</v>
+        <v>7.539191150458043e-05</v>
       </c>
       <c r="I36" t="n">
-        <v>0.336616318136387</v>
+        <v>0.4084228789259367</v>
       </c>
       <c r="J36" t="n">
-        <v>0.01870769672597524</v>
+        <v>0.009073383355506844</v>
       </c>
       <c r="K36" t="n">
-        <v>1.423232213475379e-05</v>
+        <v>4.825068715576253e-06</v>
       </c>
       <c r="L36" t="n">
-        <v>0.01795918367346939</v>
+        <v>0.012</v>
       </c>
       <c r="M36" t="n">
-        <v>108.3779296875</v>
+        <v>101.1796875</v>
       </c>
     </row>
     <row r="37">
@@ -2082,42 +2082,42 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>8096.484375</v>
+        <v>9029.296875</v>
       </c>
       <c r="E37" t="n">
-        <v>44.43852884232486</v>
+        <v>45.33487857275032</v>
       </c>
       <c r="F37" t="n">
-        <v>0.8808497642829818</v>
+        <v>0.8011721153076226</v>
       </c>
       <c r="G37" t="n">
-        <v>0.005488620342372347</v>
+        <v>0.005020864769467481</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0001087941041426368</v>
+        <v>8.873028834901639e-05</v>
       </c>
       <c r="I37" t="n">
-        <v>0.3104854512299278</v>
+        <v>0.4492337468458327</v>
       </c>
       <c r="J37" t="n">
-        <v>0.008208999747459788</v>
+        <v>0.008473784715140219</v>
       </c>
       <c r="K37" t="n">
-        <v>2.441622060815465e-06</v>
+        <v>8.687376544227353e-06</v>
       </c>
       <c r="L37" t="n">
-        <v>0.01496598639455782</v>
+        <v>0.014</v>
       </c>
       <c r="M37" t="n">
-        <v>121.171875</v>
+        <v>126.41015625</v>
       </c>
     </row>
     <row r="38">
@@ -2127,42 +2127,42 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>8484.08203125</v>
+        <v>6837.890625</v>
       </c>
       <c r="E38" t="n">
-        <v>61.50528918790371</v>
+        <v>40.14963912276762</v>
       </c>
       <c r="F38" t="n">
-        <v>1.640283419444352</v>
+        <v>1.417109964637941</v>
       </c>
       <c r="G38" t="n">
-        <v>0.007249492515673124</v>
+        <v>0.005871641025666101</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0001933365817778027</v>
+        <v>0.0002072437309039206</v>
       </c>
       <c r="I38" t="n">
-        <v>0.6894200543447602</v>
+        <v>0.2049821873672528</v>
       </c>
       <c r="J38" t="n">
-        <v>0.02362224796128088</v>
+        <v>0.009332034166856488</v>
       </c>
       <c r="K38" t="n">
-        <v>3.757761163134145e-05</v>
+        <v>4.240766410062701e-06</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0199546485260771</v>
+        <v>0.016</v>
       </c>
       <c r="M38" t="n">
-        <v>169.296875</v>
+        <v>109.40625</v>
       </c>
     </row>
     <row r="39">
@@ -2172,42 +2172,42 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>9867.59033203125</v>
+        <v>7892.578125</v>
       </c>
       <c r="E39" t="n">
-        <v>53.04578091732044</v>
+        <v>43.9350953165799</v>
       </c>
       <c r="F39" t="n">
-        <v>0.8662838466850091</v>
+        <v>0.9972192019632076</v>
       </c>
       <c r="G39" t="n">
-        <v>0.005375758329278039</v>
+        <v>0.00556663419997251</v>
       </c>
       <c r="H39" t="n">
-        <v>8.779082000120733e-05</v>
+        <v>0.0001263489807981099</v>
       </c>
       <c r="I39" t="n">
-        <v>0.2940509757305689</v>
+        <v>0.3713687639435128</v>
       </c>
       <c r="J39" t="n">
-        <v>0.005808405058633756</v>
+        <v>0.01129339804451088</v>
       </c>
       <c r="K39" t="n">
-        <v>2.610254329534449e-06</v>
+        <v>5.306494693467216e-06</v>
       </c>
       <c r="L39" t="n">
-        <v>0.01596371882086168</v>
+        <v>0.016</v>
       </c>
       <c r="M39" t="n">
-        <v>157.5234375</v>
+        <v>126.28125</v>
       </c>
     </row>
     <row r="40">
@@ -2217,42 +2217,42 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>6965.9912109375</v>
+        <v>8835.9375</v>
       </c>
       <c r="E40" t="n">
-        <v>39.35994448883449</v>
+        <v>43.38546643502074</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9692250467350343</v>
+        <v>0.6609823171074566</v>
       </c>
       <c r="G40" t="n">
-        <v>0.005650300624415707</v>
+        <v>0.004910114680532851</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0001391367025001735</v>
+        <v>7.480613314743983e-05</v>
       </c>
       <c r="I40" t="n">
-        <v>0.7654340387752829</v>
+        <v>0.4286776246064646</v>
       </c>
       <c r="J40" t="n">
-        <v>0.02813166718620787</v>
+        <v>0.008199907896277028</v>
       </c>
       <c r="K40" t="n">
-        <v>1.915298816062836e-05</v>
+        <v>3.410422038026642e-06</v>
       </c>
       <c r="L40" t="n">
-        <v>0.01696145124716553</v>
+        <v>0.014</v>
       </c>
       <c r="M40" t="n">
-        <v>118.1533203125</v>
+        <v>123.703125</v>
       </c>
     </row>
     <row r="41">
@@ -2262,42 +2262,42 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5765.51513671875</v>
+        <v>9257.8125</v>
       </c>
       <c r="E41" t="n">
-        <v>46.00619689495158</v>
+        <v>41.4833574820399</v>
       </c>
       <c r="F41" t="n">
-        <v>1.783334654870012</v>
+        <v>2.109201725132426</v>
       </c>
       <c r="G41" t="n">
-        <v>0.007979546632694207</v>
+        <v>0.004480902749114858</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0003093105494620099</v>
+        <v>0.0002278293846556544</v>
       </c>
       <c r="I41" t="n">
-        <v>0.5192789578559001</v>
+        <v>0.1542336264488695</v>
       </c>
       <c r="J41" t="n">
-        <v>0.02443369934186265</v>
+        <v>0.008834373316015833</v>
       </c>
       <c r="K41" t="n">
-        <v>5.600920060096615e-05</v>
+        <v>6.625714501257375e-06</v>
       </c>
       <c r="L41" t="n">
-        <v>0.02095238095238095</v>
+        <v>0.013</v>
       </c>
       <c r="M41" t="n">
-        <v>120.80126953125</v>
+        <v>120.3515625</v>
       </c>
     </row>
     <row r="42">
@@ -2307,42 +2307,42 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7181.3232421875</v>
+        <v>5625.54931640625</v>
       </c>
       <c r="E42" t="n">
-        <v>132.9814505584539</v>
+        <v>35.36076541626838</v>
       </c>
       <c r="F42" t="n">
-        <v>2.404688465831699</v>
+        <v>1.990375671042932</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01851768066604205</v>
+        <v>0.006285744453993654</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0003348531161645925</v>
+        <v>0.000353810011981983</v>
       </c>
       <c r="I42" t="n">
-        <v>1.224533840760661</v>
+        <v>0.3501858715691748</v>
       </c>
       <c r="J42" t="n">
-        <v>0.02237484072094962</v>
+        <v>0.02747914768057419</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0002926286435000969</v>
+        <v>2.838636867064022e-05</v>
       </c>
       <c r="L42" t="n">
-        <v>0.04589569160997732</v>
+        <v>0.01795918367346939</v>
       </c>
       <c r="M42" t="n">
-        <v>329.591796875</v>
+        <v>101.0302734375</v>
       </c>
     </row>
     <row r="43">
@@ -2352,492 +2352,492 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>9636.1083984375</v>
+        <v>8096.484375</v>
       </c>
       <c r="E43" t="n">
-        <v>99.20408562973584</v>
+        <v>44.43852884232486</v>
       </c>
       <c r="F43" t="n">
-        <v>1.980062808714697</v>
+        <v>0.8808497642829818</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01029503628724453</v>
+        <v>0.005488620342372347</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0002054836586350321</v>
+        <v>0.0001087941041426368</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9483475366464004</v>
+        <v>0.3104854512299278</v>
       </c>
       <c r="J43" t="n">
-        <v>0.0188358848966278</v>
+        <v>0.008208999747459788</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0001207782311779987</v>
+        <v>2.441622060815465e-06</v>
       </c>
       <c r="L43" t="n">
-        <v>0.02594104308390023</v>
+        <v>0.01496598639455782</v>
       </c>
       <c r="M43" t="n">
-        <v>249.970703125</v>
+        <v>121.171875</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1571.923828125</v>
+        <v>8484.08203125</v>
       </c>
       <c r="E44" t="n">
-        <v>9.327867857028981</v>
+        <v>61.50528918790371</v>
       </c>
       <c r="F44" t="n">
-        <v>0.3409387422786392</v>
+        <v>1.640283419444352</v>
       </c>
       <c r="G44" t="n">
-        <v>0.005934045715278276</v>
+        <v>0.007249492515673124</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0002168926611954938</v>
+        <v>0.0001933365817778027</v>
       </c>
       <c r="I44" t="n">
-        <v>0.684371387363926</v>
+        <v>0.6894200543447602</v>
       </c>
       <c r="J44" t="n">
-        <v>0.04859298645425911</v>
+        <v>0.02362224796128088</v>
       </c>
       <c r="K44" t="n">
-        <v>1.50510655320575e-05</v>
+        <v>3.757761163134145e-05</v>
       </c>
       <c r="L44" t="n">
-        <v>0.02095238095238095</v>
+        <v>0.0199546485260771</v>
       </c>
       <c r="M44" t="n">
-        <v>32.935546875</v>
+        <v>169.296875</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1717.27294921875</v>
+        <v>9867.59033203125</v>
       </c>
       <c r="E45" t="n">
-        <v>9.150883555178499</v>
+        <v>53.04578091732044</v>
       </c>
       <c r="F45" t="n">
-        <v>0.2714447810259077</v>
+        <v>0.8662838466850091</v>
       </c>
       <c r="G45" t="n">
-        <v>0.005328729809283708</v>
+        <v>0.005375758329278039</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0001580673480877911</v>
+        <v>8.779082000120733e-05</v>
       </c>
       <c r="I45" t="n">
-        <v>0.4349124124110318</v>
+        <v>0.2940509757305689</v>
       </c>
       <c r="J45" t="n">
-        <v>0.02480015946415856</v>
+        <v>0.005808405058633756</v>
       </c>
       <c r="K45" t="n">
-        <v>3.770456349635716e-06</v>
+        <v>2.610254329534449e-06</v>
       </c>
       <c r="L45" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.01596371882086168</v>
       </c>
       <c r="M45" t="n">
-        <v>32.55419921875</v>
+        <v>157.5234375</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1324.2919921875</v>
+        <v>4925.72021484375</v>
       </c>
       <c r="E46" t="n">
-        <v>7.603585153429194</v>
+        <v>30.2630458904727</v>
       </c>
       <c r="F46" t="n">
-        <v>0.2983849545795681</v>
+        <v>1.301160133368823</v>
       </c>
       <c r="G46" t="n">
-        <v>0.005741622843214052</v>
+        <v>0.006143882431501986</v>
       </c>
       <c r="H46" t="n">
-        <v>0.000225316589045206</v>
+        <v>0.0002641563216375451</v>
       </c>
       <c r="I46" t="n">
-        <v>0.3772582775204812</v>
+        <v>0.1428003445105029</v>
       </c>
       <c r="J46" t="n">
-        <v>0.02933079890588592</v>
+        <v>0.007754185328698305</v>
       </c>
       <c r="K46" t="n">
-        <v>4.292961686341989e-06</v>
+        <v>3.664665900857378e-06</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0199546485260771</v>
+        <v>0.01696145124716553</v>
       </c>
       <c r="M46" t="n">
-        <v>26.42578125</v>
+        <v>83.54736328125</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1566.54052734375</v>
+        <v>6965.9912109375</v>
       </c>
       <c r="E47" t="n">
-        <v>7.941382135118294</v>
+        <v>39.35994448883449</v>
       </c>
       <c r="F47" t="n">
-        <v>0.2708870669228064</v>
+        <v>0.9692250467350343</v>
       </c>
       <c r="G47" t="n">
-        <v>0.005069375478324728</v>
+        <v>0.005650300624415707</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0001729205610672113</v>
+        <v>0.0001391367025001735</v>
       </c>
       <c r="I47" t="n">
-        <v>0.4931144087769465</v>
+        <v>0.7654340387752829</v>
       </c>
       <c r="J47" t="n">
-        <v>0.03665393940243809</v>
+        <v>0.02813166718620787</v>
       </c>
       <c r="K47" t="n">
-        <v>3.318244813956831e-06</v>
+        <v>1.915298816062836e-05</v>
       </c>
       <c r="L47" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.01696145124716553</v>
       </c>
       <c r="M47" t="n">
-        <v>29.69677734375</v>
+        <v>118.1533203125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2896.2158203125</v>
+        <v>7428.955078125</v>
       </c>
       <c r="E48" t="n">
-        <v>16.86950421883625</v>
+        <v>38.31889393638549</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6877932820930341</v>
+        <v>1.299090166415778</v>
       </c>
       <c r="G48" t="n">
-        <v>0.005824670972557576</v>
+        <v>0.00515804625730175</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0002374799824202402</v>
+        <v>0.0001748684912957714</v>
       </c>
       <c r="I48" t="n">
-        <v>0.2187324483943958</v>
+        <v>0.1663153891456366</v>
       </c>
       <c r="J48" t="n">
-        <v>0.01301114995969298</v>
+        <v>0.006927109704277577</v>
       </c>
       <c r="K48" t="n">
-        <v>4.53624223206537e-06</v>
+        <v>3.075379078952301e-06</v>
       </c>
       <c r="L48" t="n">
-        <v>0.01696145124716553</v>
+        <v>0.01496598639455782</v>
       </c>
       <c r="M48" t="n">
-        <v>49.1240234375</v>
+        <v>111.181640625</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3181.53076171875</v>
+        <v>9759.92431640625</v>
       </c>
       <c r="E49" t="n">
-        <v>21.87591879261557</v>
+        <v>64.07805593607283</v>
       </c>
       <c r="F49" t="n">
-        <v>0.6091410205110586</v>
+        <v>1.623676064774597</v>
       </c>
       <c r="G49" t="n">
-        <v>0.006875909878299463</v>
+        <v>0.006565425494986557</v>
       </c>
       <c r="H49" t="n">
-        <v>0.000191461615848713</v>
+        <v>0.0001663615425834018</v>
       </c>
       <c r="I49" t="n">
-        <v>0.6442214466011325</v>
+        <v>0.0948073408103715</v>
       </c>
       <c r="J49" t="n">
-        <v>0.02391694934824499</v>
+        <v>0.002219866753363428</v>
       </c>
       <c r="K49" t="n">
-        <v>3.297045306047183e-05</v>
+        <v>1.125276944194467e-06</v>
       </c>
       <c r="L49" t="n">
-        <v>0.0199546485260771</v>
+        <v>0.01496598639455782</v>
       </c>
       <c r="M49" t="n">
-        <v>63.486328125</v>
+        <v>146.06689453125</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1108.9599609375</v>
+        <v>5765.51513671875</v>
       </c>
       <c r="E50" t="n">
-        <v>8.142290510993167</v>
+        <v>46.00619689495158</v>
       </c>
       <c r="F50" t="n">
-        <v>0.2490344343878557</v>
+        <v>1.783334654870012</v>
       </c>
       <c r="G50" t="n">
-        <v>0.007342276365063516</v>
+        <v>0.007979546632694207</v>
       </c>
       <c r="H50" t="n">
-        <v>0.0002245657581517418</v>
+        <v>0.0003093105494620099</v>
       </c>
       <c r="I50" t="n">
-        <v>0.5220355596053396</v>
+        <v>0.5192789578559001</v>
       </c>
       <c r="J50" t="n">
-        <v>0.02658238113067924</v>
+        <v>0.02443369934186265</v>
       </c>
       <c r="K50" t="n">
-        <v>1.277081181722351e-05</v>
+        <v>5.600920060096615e-05</v>
       </c>
       <c r="L50" t="n">
-        <v>0.02294784580498866</v>
+        <v>0.02095238095238095</v>
       </c>
       <c r="M50" t="n">
-        <v>25.4482421875</v>
+        <v>120.80126953125</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1329.67529296875</v>
+        <v>7181.3232421875</v>
       </c>
       <c r="E51" t="n">
-        <v>7.527460523958864</v>
+        <v>132.9814505584539</v>
       </c>
       <c r="F51" t="n">
-        <v>0.3023470409067904</v>
+        <v>2.404688465831699</v>
       </c>
       <c r="G51" t="n">
-        <v>0.005661126865907536</v>
+        <v>0.01851768066604205</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0002273841158857241</v>
+        <v>0.0003348531161645925</v>
       </c>
       <c r="I51" t="n">
-        <v>0.317584797071918</v>
+        <v>1.224533840760661</v>
       </c>
       <c r="J51" t="n">
-        <v>0.02118270437076976</v>
+        <v>0.02237484072094962</v>
       </c>
       <c r="K51" t="n">
-        <v>6.188938529059449e-06</v>
+        <v>0.0002926286435000969</v>
       </c>
       <c r="L51" t="n">
-        <v>0.01795918367346939</v>
+        <v>0.04589569160997732</v>
       </c>
       <c r="M51" t="n">
-        <v>23.8798828125</v>
+        <v>329.591796875</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2820.849609375</v>
+        <v>8833.99658203125</v>
       </c>
       <c r="E52" t="n">
-        <v>14.48467244454103</v>
+        <v>51.97048387760763</v>
       </c>
       <c r="F52" t="n">
-        <v>0.6895145947347983</v>
+        <v>1.268510604541089</v>
       </c>
       <c r="G52" t="n">
-        <v>0.005134861637572488</v>
+        <v>0.005883009280682534</v>
       </c>
       <c r="H52" t="n">
-        <v>0.0002444350781563184</v>
+        <v>0.0001435941923637708</v>
       </c>
       <c r="I52" t="n">
-        <v>0.3296372729303959</v>
+        <v>0.278733313690092</v>
       </c>
       <c r="J52" t="n">
-        <v>0.02786764506137041</v>
+        <v>0.007770308723223232</v>
       </c>
       <c r="K52" t="n">
-        <v>6.55462791341152e-06</v>
+        <v>5.919776566347984e-06</v>
       </c>
       <c r="L52" t="n">
-        <v>0.01696145124716553</v>
+        <v>0.01596371882086168</v>
       </c>
       <c r="M52" t="n">
-        <v>47.845703125</v>
+        <v>141.0234375</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>3143.84765625</v>
+        <v>9636.1083984375</v>
       </c>
       <c r="E53" t="n">
-        <v>20.46885230928134</v>
+        <v>99.20408562973584</v>
       </c>
       <c r="F53" t="n">
-        <v>0.5655495465396686</v>
+        <v>1.980062808714697</v>
       </c>
       <c r="G53" t="n">
-        <v>0.006510764689436862</v>
+        <v>0.01029503628724453</v>
       </c>
       <c r="H53" t="n">
-        <v>0.0001798908879745972</v>
+        <v>0.0002054836586350321</v>
       </c>
       <c r="I53" t="n">
-        <v>0.5838236717856504</v>
+        <v>0.9483475366464004</v>
       </c>
       <c r="J53" t="n">
-        <v>0.02214590386040583</v>
+        <v>0.0188358848966278</v>
       </c>
       <c r="K53" t="n">
-        <v>2.230499777667372e-05</v>
+        <v>0.0001207782311779987</v>
       </c>
       <c r="L53" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.02594104308390023</v>
       </c>
       <c r="M53" t="n">
-        <v>59.59765625</v>
+        <v>249.970703125</v>
       </c>
     </row>
     <row r="54">
@@ -2847,42 +2847,42 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>1103.57666015625</v>
+        <v>1184.326171875</v>
       </c>
       <c r="E54" t="n">
-        <v>8.738732929551876</v>
+        <v>5.749991376856697</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4258987788417047</v>
+        <v>0.206195271718955</v>
       </c>
       <c r="G54" t="n">
-        <v>0.007918555407210771</v>
+        <v>0.004855074145455582</v>
       </c>
       <c r="H54" t="n">
-        <v>0.0003859258665196886</v>
+        <v>0.0001741034493838054</v>
       </c>
       <c r="I54" t="n">
-        <v>0.5563368840606797</v>
+        <v>0.4355332593377296</v>
       </c>
       <c r="J54" t="n">
-        <v>0.03960055828043722</v>
+        <v>0.02899113214888388</v>
       </c>
       <c r="K54" t="n">
-        <v>6.079287035000314e-05</v>
+        <v>5.607978965453569e-06</v>
       </c>
       <c r="L54" t="n">
-        <v>0.02294784580498866</v>
+        <v>0.01696145124716553</v>
       </c>
       <c r="M54" t="n">
-        <v>25.32470703125</v>
+        <v>20.087890625</v>
       </c>
     </row>
     <row r="55">
@@ -2892,42 +2892,42 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>2287.90283203125</v>
+        <v>1571.923828125</v>
       </c>
       <c r="E55" t="n">
-        <v>13.71977695798699</v>
+        <v>9.327867857028981</v>
       </c>
       <c r="F55" t="n">
-        <v>0.4275001371009103</v>
+        <v>0.3409387422786392</v>
       </c>
       <c r="G55" t="n">
-        <v>0.005996660682397193</v>
+        <v>0.005934045715278276</v>
       </c>
       <c r="H55" t="n">
-        <v>0.000186852400860646</v>
+        <v>0.0002168926611954938</v>
       </c>
       <c r="I55" t="n">
-        <v>0.5413377653334959</v>
+        <v>0.684371387363926</v>
       </c>
       <c r="J55" t="n">
-        <v>0.02703834274282341</v>
+        <v>0.04859298645425911</v>
       </c>
       <c r="K55" t="n">
-        <v>1.372067681811912e-05</v>
+        <v>1.50510655320575e-05</v>
       </c>
       <c r="L55" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.02095238095238095</v>
       </c>
       <c r="M55" t="n">
-        <v>43.37158203125</v>
+        <v>32.935546875</v>
       </c>
     </row>
     <row r="56">
@@ -2937,42 +2937,627 @@
         </is>
       </c>
       <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>tokay_GG1rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>3219.2138671875</v>
+      </c>
+      <c r="E56" t="n">
+        <v>17.50334629248044</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.7170063626759701</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.005437149258981176</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.000222727160187835</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.4522048656247286</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0317367035725989</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1.187784794227536e-05</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.01795918367346939</v>
+      </c>
+      <c r="M56" t="n">
+        <v>57.814453125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>tokay_GG1rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>3714.4775390625</v>
+      </c>
+      <c r="E57" t="n">
+        <v>28.42886105550155</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1.057688158411817</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.007653528862817334</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.0002847474906736865</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.7275520710449699</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.04395397045938562</v>
+      </c>
+      <c r="K57" t="n">
+        <v>4.381835841279676e-05</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.02394557823129252</v>
+      </c>
+      <c r="M57" t="n">
+        <v>88.9453125</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>tokay_GG2rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1200.47607421875</v>
+      </c>
+      <c r="E58" t="n">
+        <v>6.16984324481538</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.1691044607400948</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.005139497052309528</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.0001408644989864918</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.3668787539897374</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.01975029769343536</v>
+      </c>
+      <c r="K58" t="n">
+        <v>1.829666823970551e-06</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.01795918367346939</v>
+      </c>
+      <c r="M58" t="n">
+        <v>21.5595703125</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>tokay_GG2rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1566.54052734375</v>
+      </c>
+      <c r="E59" t="n">
+        <v>7.941382135118294</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.2708870669228064</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.005069375478324728</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.0001729205610672113</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.4931144087769465</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.03665393940243809</v>
+      </c>
+      <c r="K59" t="n">
+        <v>3.318244813956831e-06</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.01895691609977324</v>
+      </c>
+      <c r="M59" t="n">
+        <v>29.69677734375</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>tokay_GG2rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>3181.53076171875</v>
+      </c>
+      <c r="E60" t="n">
+        <v>21.87591879261557</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.6091410205110586</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.006875909878299463</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.000191461615848713</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.6442214466011325</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.02391694934824499</v>
+      </c>
+      <c r="K60" t="n">
+        <v>3.297045306047183e-05</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.0199546485260771</v>
+      </c>
+      <c r="M60" t="n">
+        <v>63.486328125</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>tokay_GG2rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>3875.9765625</v>
+      </c>
+      <c r="E61" t="n">
+        <v>23.25342466700442</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1.077939435215253</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.005999371846564004</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.0002781078311061777</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.3373664306228514</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.02231637889335208</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1.469021165454178e-05</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.01696145124716553</v>
+      </c>
+      <c r="M61" t="n">
+        <v>65.7421875</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>tokay_GG3rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1108.9599609375</v>
+      </c>
+      <c r="E62" t="n">
+        <v>8.142290510993167</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.2490344343878557</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.007342276365063516</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.0002245657581517418</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.5220355596053396</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.02658238113067924</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1.277081181722351e-05</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.02294784580498866</v>
+      </c>
+      <c r="M62" t="n">
+        <v>25.4482421875</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>tokay_GG3rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1620.37353515625</v>
+      </c>
+      <c r="E63" t="n">
+        <v>9.245652514882419</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.6117033916493099</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.005705877264893046</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.0003775076415268189</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.2205159618135425</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.02382981401503815</v>
+      </c>
+      <c r="K63" t="n">
+        <v>7.20872448923846e-06</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.01696145124716553</v>
+      </c>
+      <c r="M63" t="n">
+        <v>27.48388671875</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>tokay_GG3rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>2271.7529296875</v>
+      </c>
+      <c r="E64" t="n">
+        <v>12.41537097454172</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.5885702075197421</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.005465106179592149</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.0002590819625797534</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.2750485513274818</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.02225112700589143</v>
+      </c>
+      <c r="K64" t="n">
+        <v>5.958193541439499e-06</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.01795918367346939</v>
+      </c>
+      <c r="M64" t="n">
+        <v>40.798828125</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>tokay_GG3rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>3143.84765625</v>
+      </c>
+      <c r="E65" t="n">
+        <v>20.46885230928134</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.5655495465396686</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.006510764689436862</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.0001798908879745972</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.5838236717856504</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.02214590386040583</v>
+      </c>
+      <c r="K65" t="n">
+        <v>2.230499777667372e-05</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.01895691609977324</v>
+      </c>
+      <c r="M65" t="n">
+        <v>59.59765625</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
         <v>3</v>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D66" t="n">
+        <v>1103.57666015625</v>
+      </c>
+      <c r="E66" t="n">
+        <v>8.738732929551876</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.4258987788417047</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.007918555407210771</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.0003859258665196886</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.5563368840606797</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.03960055828043722</v>
+      </c>
+      <c r="K66" t="n">
+        <v>6.079287035000314e-05</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.02294784580498866</v>
+      </c>
+      <c r="M66" t="n">
+        <v>25.32470703125</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>tokay_GG4rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2287.90283203125</v>
+      </c>
+      <c r="E67" t="n">
+        <v>13.71977695798699</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.4275001371009103</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.005996660682397193</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.000186852400860646</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.5413377653334959</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.02703834274282341</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1.372067681811912e-05</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0.01895691609977324</v>
+      </c>
+      <c r="M67" t="n">
+        <v>43.37158203125</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>tokay_GG4rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
         <v>3159.99755859375</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E68" t="n">
         <v>19.47528584746784</v>
       </c>
-      <c r="F56" t="n">
+      <c r="F68" t="n">
         <v>0.5708999106909342</v>
       </c>
-      <c r="G56" t="n">
+      <c r="G68" t="n">
         <v>0.00616306990317254</v>
       </c>
-      <c r="H56" t="n">
+      <c r="H68" t="n">
         <v>0.000180664668280628</v>
       </c>
-      <c r="I56" t="n">
+      <c r="I68" t="n">
         <v>0.4205915749115395</v>
       </c>
-      <c r="J56" t="n">
+      <c r="J68" t="n">
         <v>0.01553763150729568</v>
       </c>
-      <c r="K56" t="n">
+      <c r="K68" t="n">
         <v>1.484367197319866e-05</v>
       </c>
-      <c r="L56" t="n">
+      <c r="L68" t="n">
         <v>0.01696145124716553</v>
       </c>
-      <c r="M56" t="n">
+      <c r="M68" t="n">
         <v>53.59814453125</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Tokay</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>tokay_GG4rearSOAEwf.mat</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>2847.76611328125</v>
+      </c>
+      <c r="E69" t="n">
+        <v>16.31249086797613</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.7744673567878769</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.005728170860626109</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.0002719560968072343</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.3142827976271799</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.024553023437913</v>
+      </c>
+      <c r="K69" t="n">
+        <v>8.693537059254071e-06</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.01795918367346939</v>
+      </c>
+      <c r="M69" t="n">
+        <v>51.1435546875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>